<commit_message>
analyse korte eiwitten 3
</commit_message>
<xml_diff>
--- a/code/resultskort/ANALYSIS/analyze2_14_9_erroredit.xlsx
+++ b/code/resultskort/ANALYSIS/analyze2_14_9_erroredit.xlsx
@@ -7921,8 +7921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>